<commit_message>
Add second factor to 0-var baseline-inv. fixture
Test passes.
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/stata_results/basic_2f/basic_2f.xlsx
+++ b/tests/testthat/fixtures/stata_results/basic_2f/basic_2f.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="24" uniqueCount="16">
   <si>
     <t>ln_real_wage</t>
   </si>
@@ -51,6 +51,12 @@
     <t>advanced_degree</t>
   </si>
   <si>
+    <t>foreign_born</t>
+  </si>
+  <si>
+    <t>native</t>
+  </si>
+  <si>
     <t>Intercept</t>
   </si>
   <si>
@@ -65,7 +71,87 @@
     <numFmt numFmtId="166" formatCode="0.######"/>
     <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
-  <fonts count="104">
+  <fonts count="124">
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -491,7 +577,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="104">
+  <borders count="124">
     <border>
       <left/>
       <right/>
@@ -1189,6 +1275,146 @@
       <left style="none"/>
       <right style="none"/>
       <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
       <bottom style="thin"/>
       <diagonal style="none"/>
     </border>
@@ -1224,7 +1450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -1618,23 +1844,103 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="99" fillId="0" borderId="99" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="100" fillId="0" borderId="100" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="101" fillId="0" borderId="101" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="102" fillId="0" borderId="102" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="103" fillId="0" borderId="103" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="99" fillId="0" borderId="99" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="100" fillId="0" borderId="100" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="101" fillId="0" borderId="101" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="102" fillId="0" borderId="102" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="103" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="104" fillId="0" borderId="104" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="105" fillId="0" borderId="105" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="106" fillId="0" borderId="106" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="107" fillId="0" borderId="107" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="108" fillId="0" borderId="108" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="109" fillId="0" borderId="109" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="110" fillId="0" borderId="110" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="111" fillId="0" borderId="111" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="112" fillId="0" borderId="112" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="113" fillId="0" borderId="113" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="114" fillId="0" borderId="114" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="115" fillId="0" borderId="115" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="116" fillId="0" borderId="116" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="117" fillId="0" borderId="117" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="118" fillId="0" borderId="118" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="119" fillId="0" borderId="119" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="120" fillId="0" borderId="120" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="121" fillId="0" borderId="121" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="122" fillId="0" borderId="122" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="123" fillId="0" borderId="123" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1647,7 +1953,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1688,7 +1994,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="26">
-        <v>-0.028940479294251809</v>
+        <v>-0.032271001107906816</v>
       </c>
     </row>
     <row r="6">
@@ -1696,7 +2002,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="31">
-        <v>0.2348752232874336</v>
+        <v>0.23820574510108861</v>
       </c>
     </row>
     <row r="7">
@@ -1704,7 +2010,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="36">
-        <v>0.012347954981222771</v>
+        <v>0.013535905928788528</v>
       </c>
     </row>
     <row r="8">
@@ -1712,7 +2018,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="41">
-        <v>-0.029677235014995033</v>
+        <v>-0.027896418940767151</v>
       </c>
     </row>
     <row r="9">
@@ -1720,7 +2026,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="46">
-        <v>0.0050367059543874812</v>
+        <v>0.0061831203212692615</v>
       </c>
     </row>
     <row r="10">
@@ -1728,7 +2034,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="51">
-        <v>-0.00057333166967538638</v>
+        <v>-0.00054999728234909873</v>
       </c>
     </row>
     <row r="11">
@@ -1736,7 +2042,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="56">
-        <v>-0.0048623828936868261</v>
+        <v>-0.004643640712819158</v>
       </c>
     </row>
     <row r="12">
@@ -1744,70 +2050,102 @@
         <v>11</v>
       </c>
       <c r="B12" s="61">
-        <v>-0.011212190651504764</v>
+        <v>-0.010966301720579542</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="63" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B13" s="66">
-        <v>-0.067617083991683424</v>
+        <v>-0.0039668343507246878</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="68" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B14" s="71">
-        <v>-0.024526288550055817</v>
+        <v>-0.0039668343507246904</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="73" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B15" s="76">
-        <v>0.0091238244284653196</v>
+        <v>-0.032635916559729472</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="78" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B16" s="81">
-        <v>-0.0058998531903625617</v>
+        <v>-0.016742719617206386</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="83" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B17" s="86">
-        <v>0.0063995418212052929</v>
+        <v>0.003649280982492543</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="88" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B18" s="91">
-        <v>0.0047374082412474858</v>
+        <v>-0.0067544010924489653</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="96">
+        <v>0.0071334101898753001</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="101">
+        <v>0.0046010329652941655</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="96">
-        <v>0.3126576745286167</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="99" t="s">
+      <c r="B21" s="106">
+        <v>-0.023953816220072303</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="103">
+      <c r="B22" s="111">
+        <v>0.019059210963953077</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="116">
+        <v>0.28384966348893004</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="119" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="123">
         <v>666</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tests against Stata for baseline-invariant results with more than one factor IV (#56)
* Add second factor to 0-var baseline-invariant test

Updates both test and fixture, with a sort disabled in the test to demo that the test can fail.

* Un-break new test

* Add second factor to twofold baseline-invariant test

Fixture not yet updated, test fails.

* Add second factor to 0-var baseline-inv. fixture

Test passes.

* Add second factor to threefold baseline-invariant test

Fixture not yet updated, test fails.

* Add second factor to 0-var baseline-inv. fixture

Test passes.
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/stata_results/basic_2f/basic_2f.xlsx
+++ b/tests/testthat/fixtures/stata_results/basic_2f/basic_2f.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="24" uniqueCount="16">
   <si>
     <t>ln_real_wage</t>
   </si>
@@ -51,6 +51,12 @@
     <t>advanced_degree</t>
   </si>
   <si>
+    <t>foreign_born</t>
+  </si>
+  <si>
+    <t>native</t>
+  </si>
+  <si>
     <t>Intercept</t>
   </si>
   <si>
@@ -65,7 +71,87 @@
     <numFmt numFmtId="166" formatCode="0.######"/>
     <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
-  <fonts count="104">
+  <fonts count="124">
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -491,7 +577,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="104">
+  <borders count="124">
     <border>
       <left/>
       <right/>
@@ -1189,6 +1275,146 @@
       <left style="none"/>
       <right style="none"/>
       <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
       <bottom style="thin"/>
       <diagonal style="none"/>
     </border>
@@ -1224,7 +1450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -1618,23 +1844,103 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="99" fillId="0" borderId="99" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="100" fillId="0" borderId="100" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="101" fillId="0" borderId="101" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="102" fillId="0" borderId="102" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="103" fillId="0" borderId="103" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="99" fillId="0" borderId="99" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="100" fillId="0" borderId="100" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="101" fillId="0" borderId="101" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="102" fillId="0" borderId="102" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="103" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="104" fillId="0" borderId="104" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="105" fillId="0" borderId="105" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="106" fillId="0" borderId="106" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="107" fillId="0" borderId="107" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="108" fillId="0" borderId="108" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="109" fillId="0" borderId="109" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="110" fillId="0" borderId="110" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="111" fillId="0" borderId="111" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="112" fillId="0" borderId="112" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="113" fillId="0" borderId="113" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="114" fillId="0" borderId="114" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="115" fillId="0" borderId="115" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="116" fillId="0" borderId="116" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="117" fillId="0" borderId="117" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="118" fillId="0" borderId="118" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="119" fillId="0" borderId="119" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="120" fillId="0" borderId="120" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="121" fillId="0" borderId="121" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="122" fillId="0" borderId="122" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="123" fillId="0" borderId="123" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1647,7 +1953,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1688,7 +1994,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="26">
-        <v>-0.028940479294251809</v>
+        <v>-0.032271001107906816</v>
       </c>
     </row>
     <row r="6">
@@ -1696,7 +2002,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="31">
-        <v>0.2348752232874336</v>
+        <v>0.23820574510108861</v>
       </c>
     </row>
     <row r="7">
@@ -1704,7 +2010,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="36">
-        <v>0.012347954981222771</v>
+        <v>0.013535905928788528</v>
       </c>
     </row>
     <row r="8">
@@ -1712,7 +2018,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="41">
-        <v>-0.029677235014995033</v>
+        <v>-0.027896418940767151</v>
       </c>
     </row>
     <row r="9">
@@ -1720,7 +2026,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="46">
-        <v>0.0050367059543874812</v>
+        <v>0.0061831203212692615</v>
       </c>
     </row>
     <row r="10">
@@ -1728,7 +2034,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="51">
-        <v>-0.00057333166967538638</v>
+        <v>-0.00054999728234909873</v>
       </c>
     </row>
     <row r="11">
@@ -1736,7 +2042,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="56">
-        <v>-0.0048623828936868261</v>
+        <v>-0.004643640712819158</v>
       </c>
     </row>
     <row r="12">
@@ -1744,70 +2050,102 @@
         <v>11</v>
       </c>
       <c r="B12" s="61">
-        <v>-0.011212190651504764</v>
+        <v>-0.010966301720579542</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="63" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B13" s="66">
-        <v>-0.067617083991683424</v>
+        <v>-0.0039668343507246878</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="68" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B14" s="71">
-        <v>-0.024526288550055817</v>
+        <v>-0.0039668343507246904</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="73" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B15" s="76">
-        <v>0.0091238244284653196</v>
+        <v>-0.032635916559729472</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="78" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B16" s="81">
-        <v>-0.0058998531903625617</v>
+        <v>-0.016742719617206386</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="83" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B17" s="86">
-        <v>0.0063995418212052929</v>
+        <v>0.003649280982492543</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="88" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B18" s="91">
-        <v>0.0047374082412474858</v>
+        <v>-0.0067544010924489653</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="96">
+        <v>0.0071334101898753001</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="101">
+        <v>0.0046010329652941655</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="96">
-        <v>0.3126576745286167</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="99" t="s">
+      <c r="B21" s="106">
+        <v>-0.023953816220072303</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="103">
+      <c r="B22" s="111">
+        <v>0.019059210963953077</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="116">
+        <v>0.28384966348893004</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="119" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="123">
         <v>666</v>
       </c>
     </row>

</xml_diff>